<commit_message>
correcting smote, running cluster analysis
</commit_message>
<xml_diff>
--- a/data/uniques_OLS.xlsx
+++ b/data/uniques_OLS.xlsx
@@ -451,27 +451,27 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>494</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>201</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>342</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>410</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>799</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>494</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>201</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>410</t>
         </is>
       </c>
     </row>
@@ -584,13 +584,13 @@
         <v>0.02203759613901316</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.002203759613901316</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.002203759613901316</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -624,10 +624,10 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>0.00184060371801951</v>
       </c>
       <c r="I6" t="n">
-        <v>0.00184060371801951</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -928,13 +928,13 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>0.00962186086789185</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>0.00962186086789185</v>
+        <v>0</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
@@ -959,13 +959,13 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>0.01465774173059071</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>0.01465774173059071</v>
+        <v>0</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -1114,13 +1114,13 @@
         <v>0</v>
       </c>
       <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
         <v>0.002372948388372553</v>
-      </c>
-      <c r="G22" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" t="n">
-        <v>0</v>
       </c>
       <c r="I22" t="n">
         <v>0.002372948388372553</v>
@@ -1145,13 +1145,13 @@
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>0.01529597715800744</v>
       </c>
       <c r="G23" t="n">
         <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>0.01529597715800744</v>
+        <v>0</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
@@ -1266,19 +1266,19 @@
         <v>0</v>
       </c>
       <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
         <v>0.00395872370747671</v>
       </c>
-      <c r="F27" t="n">
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
         <v>0.001319574569158903</v>
-      </c>
-      <c r="G27" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1545,13 +1545,13 @@
         <v>0</v>
       </c>
       <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
         <v>0.003618206816701643</v>
-      </c>
-      <c r="F36" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" t="n">
-        <v>0</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
@@ -2289,13 +2289,13 @@
         <v>0.003503485968538696</v>
       </c>
       <c r="E60" t="n">
-        <v>0</v>
+        <v>0.003503485968538696</v>
       </c>
       <c r="F60" t="n">
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>0.003503485968538696</v>
+        <v>0</v>
       </c>
       <c r="H60" t="n">
         <v>0</v>

</xml_diff>